<commit_message>
UPDATE: info_sensores ahora tiene más información
</commit_message>
<xml_diff>
--- a/sensores_y_actuadores/info_sensores.xlsx
+++ b/sensores_y_actuadores/info_sensores.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\serwikk\Domotica\sensores_y_actuadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7378B-255E-4ED0-87AB-1D353D9A6F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2090254C-9A73-41DE-87A9-D50FA710389B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EDA9BEC-467A-4CB5-A0AD-421B493A575A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0EDA9BEC-467A-4CB5-A0AD-421B493A575A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensores" sheetId="1" r:id="rId1"/>
+    <sheet name="Actuadores" sheetId="5" r:id="rId2"/>
+    <sheet name="Temperatura" sheetId="2" r:id="rId3"/>
+    <sheet name="Humedad" sheetId="4" r:id="rId4"/>
+    <sheet name="Luz" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t>archivo</t>
   </si>
@@ -120,13 +124,163 @@
   </si>
   <si>
     <t>cont-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       </t>
+  </si>
+  <si>
+    <t>SENSOR DE HUMEDAD</t>
+  </si>
+  <si>
+    <t>Mínimo</t>
+  </si>
+  <si>
+    <t>Máximo</t>
+  </si>
+  <si>
+    <t>Habitáculos</t>
+  </si>
+  <si>
+    <t>Dormitorio</t>
+  </si>
+  <si>
+    <t>Sala</t>
+  </si>
+  <si>
+    <t>Cocina</t>
+  </si>
+  <si>
+    <t>Baño</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Elementos que hacen bajar la humedad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elementos que hacen subir la humedad</t>
+  </si>
+  <si>
+    <t>Abrir ventanas, extractor</t>
+  </si>
+  <si>
+    <t>Plantas de interior, humidificador</t>
+  </si>
+  <si>
+    <t>Cocinar, hervir agua</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ducharse, baño caliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>ACTUADORES</t>
+  </si>
+  <si>
+    <t>Persiana</t>
+  </si>
+  <si>
+    <t>Actuadores</t>
+  </si>
+  <si>
+    <t>Efectos</t>
+  </si>
+  <si>
+    <t>Apertura ventana</t>
+  </si>
+  <si>
+    <t>Radiador</t>
+  </si>
+  <si>
+    <t>Aire acondicionado</t>
+  </si>
+  <si>
+    <t>Humidificador</t>
+  </si>
+  <si>
+    <t>Deshumidificador</t>
+  </si>
+  <si>
+    <t>Abrir ventanas, aire acondicionado, deshumidificador</t>
+  </si>
+  <si>
+    <t>Dormitorio, sala, baño, cocina</t>
+  </si>
+  <si>
+    <t>Extractor</t>
+  </si>
+  <si>
+    <t>Baño, cocina</t>
+  </si>
+  <si>
+    <t>Temperatura</t>
+  </si>
+  <si>
+    <t>Humedad</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Aumenta</t>
+  </si>
+  <si>
+    <t>Si T ext &gt;, aumenta; Si T ext &lt;, baja</t>
+  </si>
+  <si>
+    <t>Disminuye</t>
+  </si>
+  <si>
+    <t>Disminuye*</t>
+  </si>
+  <si>
+    <t>* Disminuye si se hace corriente</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Encender</t>
+  </si>
+  <si>
+    <t>Levantar</t>
+  </si>
+  <si>
+    <t>Abrir</t>
+  </si>
+  <si>
+    <t>Aumenta (por el compresor)</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Leyenda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +302,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +345,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -267,22 +516,249 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,6 +792,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFA3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -663,10 +1144,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5342F615-871D-45B7-B0D2-F6493FECE971}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.89999084444715716"/>
+  </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,20 +1165,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -729,13 +1213,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="4"/>
@@ -848,22 +1332,27 @@
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
     </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
     </row>
   </sheetData>
@@ -877,4 +1366,624 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681C110D-4B92-4A48-BE8A-EA1EA6D238DA}">
+  <sheetPr>
+    <tabColor rgb="FFFFFFA3"/>
+  </sheetPr>
+  <dimension ref="B3:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="44">
+        <v>0.6</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="45">
+        <v>1</v>
+      </c>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="P7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="50">
+        <v>0.6</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="47">
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="45">
+        <v>1</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="25">
+        <v>0</v>
+      </c>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="49">
+        <v>1</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="25">
+        <v>0</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="45">
+        <v>1</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="25">
+        <v>0</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="49">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="47">
+        <v>0.6</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="M17" s="30"/>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="41"/>
+      <c r="M19" s="32">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="42"/>
+      <c r="M20" s="33">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="43"/>
+      <c r="M22" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="36">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="41"/>
+      <c r="M24" s="37">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="42"/>
+      <c r="M25" s="38">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="42"/>
+      <c r="M26" s="39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="42"/>
+      <c r="M27" s="40">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="C3:N4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7CD8DD-C1D7-4892-AA5B-0AD57674F1D1}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9886B81E-3956-4037-B604-3F5264FC3586}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="6" max="6" width="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="12">
+        <v>30</v>
+      </c>
+      <c r="E6" s="12">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="12">
+        <v>30</v>
+      </c>
+      <c r="E7" s="12">
+        <v>50</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="12">
+        <v>30</v>
+      </c>
+      <c r="E8" s="12">
+        <v>60</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="12">
+        <v>30</v>
+      </c>
+      <c r="E9" s="12">
+        <v>70</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD69003B-8DEE-4626-910B-C4AE023EF256}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>